<commit_message>
feat: commit changes from Paul & Katy
</commit_message>
<xml_diff>
--- a/data/excel_dumps/patients/patient_0.xlsx
+++ b/data/excel_dumps/patients/patient_0.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Student Id</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>2019-12-05</t>
+  </si>
+  <si>
+    <t>2019-12-24</t>
+  </si>
+  <si>
+    <t>asklyarova@stonybrook.edu</t>
+  </si>
+  <si>
+    <t>2019-12-26</t>
+  </si>
+  <si>
+    <t>2019-12-30</t>
   </si>
 </sst>
 </file>
@@ -395,7 +407,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -622,6 +634,125 @@
       </c>
       <c r="E13" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>248</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>298</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>123</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>